<commit_message>
Including draft 1 of cooking
</commit_message>
<xml_diff>
--- a/tables/Section-19/cooking-sccs.xlsx
+++ b/tables/Section-19/cooking-sccs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/seltzer_karl_epa_gov1/Documents/Profile/Documents/GitHub/EIAG_TSD/tables/Section-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{2DD9D2DD-9371-4967-916F-8EB18BCEDA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1165DA53-B87A-4623-AA5B-6F37204D5845}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{2DD9D2DD-9371-4967-916F-8EB18BCEDA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B3EF95C-0E85-4F5B-AA70-8B0580AA24C6}"/>
   <bookViews>
-    <workbookView xWindow="1467" yWindow="1467" windowWidth="19200" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9675" yWindow="1215" windowWidth="17745" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,9 @@
     <t>SCC</t>
   </si>
   <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>SCC Level 1</t>
   </si>
   <si>
@@ -45,68 +48,65 @@
     <t>SCC Level 4</t>
   </si>
   <si>
-    <t>EPA</t>
+    <t>Estimated by EPA?</t>
+  </si>
+  <si>
+    <t>Industrial Processes</t>
+  </si>
+  <si>
+    <t>Food and Kindred Products: SIC 20</t>
+  </si>
+  <si>
+    <t>Commercial Cooking - Charbroiling</t>
+  </si>
+  <si>
+    <t>Charbroiling Total</t>
+  </si>
+  <si>
+    <t>Commercial Cooking – Charbroiling</t>
+  </si>
+  <si>
+    <t>Conveyorized Charbroiling</t>
+  </si>
+  <si>
+    <t>Under-fired Charbroiling</t>
+  </si>
+  <si>
+    <t>Commercial Cooking - Frying</t>
+  </si>
+  <si>
+    <t>Deep Fat Frying</t>
+  </si>
+  <si>
+    <t>Commercial Cooking – Frying</t>
+  </si>
+  <si>
+    <t>Flat Griddle Frying</t>
+  </si>
+  <si>
+    <t>Clamshell Griddle Frying</t>
+  </si>
+  <si>
+    <t>Miscellaneous Area Sources</t>
+  </si>
+  <si>
+    <t>Residential Cooking - Total</t>
+  </si>
+  <si>
+    <t>Other Combustion</t>
+  </si>
+  <si>
+    <t>Residential Grilling</t>
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Industrial Processes</t>
-  </si>
-  <si>
-    <t>Food and Kindred Products: SIC 20</t>
-  </si>
-  <si>
-    <t>Commercial Cooking - Charbroiling</t>
-  </si>
-  <si>
-    <t>Charbroiling Total</t>
-  </si>
-  <si>
-    <t>Commercial Cooking – Charbroiling</t>
-  </si>
-  <si>
-    <t>Conveyorized Charbroiling</t>
-  </si>
-  <si>
-    <t>Under-fired Charbroiling</t>
-  </si>
-  <si>
-    <t>Commercial Cooking - Frying</t>
-  </si>
-  <si>
-    <t>Deep Fat Frying</t>
-  </si>
-  <si>
-    <t>Commercial Cooking – Frying</t>
-  </si>
-  <si>
-    <t>Flat Griddle Frying</t>
-  </si>
-  <si>
-    <t>Clamshell Griddle Frying</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Miscellaneous Area Sources</t>
-  </si>
-  <si>
-    <t>Residential Cooking - Total</t>
-  </si>
-  <si>
-    <t>Other Combustion</t>
-  </si>
-  <si>
-    <t>Residential Grilling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,15 +116,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -138,12 +130,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -155,13 +153,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -172,7 +183,9 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -185,22 +198,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -210,30 +208,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -516,194 +502,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="39.5859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>2302002000</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2302002100</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2302002200</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>2302003000</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>2302003100</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>2302003200</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>2812001000</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5">
-        <v>2302002000</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="7">
-        <v>2302002100</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="7">
-        <v>2302002200</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="7">
-        <v>2302003000</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="7">
-        <v>2302003100</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="7">
-        <v>2302003200</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="7">
-        <v>2812001000</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="F8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>2810025000</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="7">
-        <v>2810025000</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="8"/>
-    </row>
+      <c r="E9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>